<commit_message>
Even More Part Orders
$$$$$$$$
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
   <si>
     <t>Parts for Senior Design</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/wurth-electronics-inc/744771147/732-1214-1-ND/1639275</t>
+  </si>
+  <si>
+    <t>Above Atmospheric</t>
   </si>
 </sst>
 </file>
@@ -1560,10 +1563,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P48"/>
+  <dimension ref="B3:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,7 +1577,7 @@
     <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>52</v>
       </c>
@@ -1584,7 +1587,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>25</v>
       </c>
@@ -1598,7 +1601,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>53</v>
       </c>
@@ -1612,7 +1615,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>54</v>
       </c>
@@ -1626,7 +1629,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>57</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>56</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>3.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>58</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>59</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>61</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>66</v>
       </c>
@@ -1678,7 +1681,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>48</v>
       </c>
@@ -1686,7 +1689,23 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <f>1/(1000000)</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="17" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <f>500000</f>
+        <v>500000</v>
+      </c>
+      <c r="R17">
+        <f>R16*Q17</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M33" t="s">
         <v>68</v>
       </c>
@@ -1696,8 +1715,16 @@
       <c r="O33" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="R33">
+        <f>1645-1635</f>
+        <v>10</v>
+      </c>
+      <c r="T33">
+        <f>R33*R34</f>
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M34" t="s">
         <v>69</v>
       </c>
@@ -1707,8 +1734,16 @@
       <c r="O34" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="R34">
+        <f>150-1</f>
+        <v>149</v>
+      </c>
+      <c r="T34">
+        <f>T33/R35</f>
+        <v>0.11367971313038834</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M35" t="s">
         <v>70</v>
       </c>
@@ -1721,8 +1756,19 @@
       <c r="P35" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="R35">
+        <f>14745-1638</f>
+        <v>13107</v>
+      </c>
+      <c r="T35">
+        <f>T34+1</f>
+        <v>1.1136797131303884</v>
+      </c>
+      <c r="U35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M36" t="s">
         <v>71</v>
       </c>
@@ -1736,7 +1782,40 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R37">
+        <f>1673-1635</f>
+        <v>38</v>
+      </c>
+      <c r="T37">
+        <f>R37*R38</f>
+        <v>5662</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R38">
+        <f>150-1</f>
+        <v>149</v>
+      </c>
+      <c r="T38">
+        <f>T37/R39</f>
+        <v>0.43198290989547572</v>
+      </c>
+    </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R39">
+        <f>14745-1638</f>
+        <v>13107</v>
+      </c>
+      <c r="T39">
+        <f>T38+1</f>
+        <v>1.4319829098954757</v>
+      </c>
+      <c r="U39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
New Parts and Pressure Table
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -1565,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,7 +1577,7 @@
     <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>52</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>25</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>53</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>54</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>57</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>56</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>3.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>58</v>
       </c>
@@ -1657,23 +1657,31 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>59</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T10">
+        <f>1.5688/12</f>
+        <v>0.13073333333333334</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>61</v>
       </c>
       <c r="C11" s="4">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <f>M18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>66</v>
       </c>
@@ -1681,7 +1689,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>48</v>
       </c>
@@ -1689,13 +1697,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="R16">
         <f>1/(1000000)</f>
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="17" spans="17:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="13:18" x14ac:dyDescent="0.25">
       <c r="Q17">
         <f>500000</f>
         <v>500000</v>
@@ -1703,6 +1711,11 @@
       <c r="R17">
         <f>R16*Q17</f>
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding Data Sheets for Parts
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -1565,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,7 +1852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C26:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>

</xml_diff>